<commit_message>
update child growth failure output shell data
</commit_message>
<xml_diff>
--- a/docs/source/concept_models/vivarium_gates_bep/BEP_output_shell_metadata_24July2020.xlsx
+++ b/docs/source/concept_models/vivarium_gates_bep/BEP_output_shell_metadata_24July2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\vivarium_research\docs\source\gbd2017_models\concept_models\vivarium_gates_bep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibow\vivarium_research\docs\source\concept_models\vivarium_gates_bep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
   <si>
     <t>Outcome</t>
   </si>
@@ -300,12 +300,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Mean child WLZ </t>
-  </si>
-  <si>
-    <t>Mean child LAZ</t>
-  </si>
-  <si>
     <t>Covered, low BMI mothers, at 0-7 days, 7-28 days, 28 days - 6 months, 6 months -1 year, 1-2 year</t>
   </si>
   <si>
@@ -352,6 +346,18 @@
   </si>
   <si>
     <t>F(iii)</t>
+  </si>
+  <si>
+    <t>Mean child WLZ at 29 days and 366 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This outcome is not subject to standard age group stratification, but rather should be observed at 29 and 366 days specifically </t>
+  </si>
+  <si>
+    <t>Mean child LAZ at 29 days and 366 days</t>
+  </si>
+  <si>
+    <t>This outcome is not subject to standard age group stratification, but rather should be observed at birth only</t>
   </si>
 </sst>
 </file>
@@ -808,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -833,7 +839,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -852,13 +858,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>8</v>
@@ -872,13 +878,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>9</v>
@@ -897,13 +903,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>10</v>
@@ -917,10 +923,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>11</v>
@@ -931,7 +937,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>12</v>
@@ -942,7 +948,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>13</v>
@@ -953,7 +959,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>63</v>
@@ -964,7 +970,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>64</v>
@@ -975,18 +981,18 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="E10" s="9" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="E11" s="9" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -994,7 +1000,7 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">

</xml_diff>